<commit_message>
Update AN-method output (only mundist).xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/AN-method output (only mundist).xlsx
+++ b/migforecasting/clustering/AN-method output (only mundist).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>clust</t>
   </si>
@@ -4035,8 +4035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5105,6 +5105,9 @@
       <c r="N20" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="O20" s="28" t="s">
+        <v>23</v>
+      </c>
       <c r="P20" s="10" t="s">
         <v>22</v>
       </c>
@@ -5179,67 +5182,67 @@
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="15">
-        <f>(C2/C3)-1</f>
+        <f t="shared" ref="C25:R25" si="0">(C2/C3)-1</f>
         <v>2.2364226635940065E-2</v>
       </c>
       <c r="D25" s="15">
-        <f>(D2/D3)-1</f>
+        <f t="shared" si="0"/>
         <v>-4.5743197755307441E-2</v>
       </c>
       <c r="E25" s="15">
-        <f>(E2/E3)-1</f>
+        <f t="shared" si="0"/>
         <v>2.7774349516331842E-2</v>
       </c>
       <c r="F25" s="15">
-        <f>(F2/F3)-1</f>
+        <f t="shared" si="0"/>
         <v>5.3474901878183267E-3</v>
       </c>
       <c r="G25" s="15">
-        <f>(G2/G3)-1</f>
+        <f t="shared" si="0"/>
         <v>0.14461645276441581</v>
       </c>
       <c r="H25" s="15">
-        <f>(H2/H3)-1</f>
+        <f t="shared" si="0"/>
         <v>9.9704416197773149E-2</v>
       </c>
       <c r="I25" s="15">
-        <f>(I2/I3)-1</f>
+        <f t="shared" si="0"/>
         <v>6.6799773221124736E-2</v>
       </c>
       <c r="J25" s="15">
-        <f>(J2/J3)-1</f>
+        <f t="shared" si="0"/>
         <v>-8.6941013784360033E-2</v>
       </c>
       <c r="K25" s="15">
-        <f>(K2/K3)-1</f>
+        <f t="shared" si="0"/>
         <v>2.4699306072995864E-2</v>
       </c>
       <c r="L25" s="15">
-        <f>(L2/L3)-1</f>
+        <f t="shared" si="0"/>
         <v>-3.8789332453257219E-2</v>
       </c>
       <c r="M25" s="15">
-        <f>(M2/M3)-1</f>
+        <f t="shared" si="0"/>
         <v>0.13749994095015872</v>
       </c>
       <c r="N25" s="15">
-        <f>(N2/N3)-1</f>
+        <f t="shared" si="0"/>
         <v>0.25861368569064869</v>
       </c>
       <c r="O25" s="15">
-        <f>(O2/O3)-1</f>
+        <f t="shared" si="0"/>
         <v>0.20980388556349383</v>
       </c>
       <c r="P25" s="15">
-        <f>(P2/P3)-1</f>
+        <f t="shared" si="0"/>
         <v>-0.10010439308011876</v>
       </c>
       <c r="Q25" s="15">
-        <f>(Q2/Q3)-1</f>
+        <f t="shared" si="0"/>
         <v>-0.1785524891387561</v>
       </c>
       <c r="R25" s="15">
-        <f>(R2/R3)-1</f>
+        <f t="shared" si="0"/>
         <v>0.19480529083602205</v>
       </c>
     </row>
@@ -5253,63 +5256,63 @@
         <v>0.21094715575120637</v>
       </c>
       <c r="D26" s="15">
-        <f t="shared" ref="D26:R26" si="0">(D5/D6)-1</f>
+        <f t="shared" ref="D26:R26" si="1">(D5/D6)-1</f>
         <v>3.0509624868235496E-2</v>
       </c>
       <c r="E26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.438993738363342E-2</v>
       </c>
       <c r="F26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1978388733416834E-2</v>
       </c>
       <c r="G26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.3145081627309381E-3</v>
       </c>
       <c r="H26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.16127795903622766</v>
       </c>
       <c r="I26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9608327240562282E-2</v>
       </c>
       <c r="J26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.8922843263540248E-2</v>
       </c>
       <c r="K26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3503011526366802E-2</v>
       </c>
       <c r="L26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.5160987023170396E-2</v>
       </c>
       <c r="M26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.4709366162986717E-2</v>
       </c>
       <c r="N26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3761624816903248E-2</v>
       </c>
       <c r="O26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1230402599800573</v>
       </c>
       <c r="P26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.16355901877733359</v>
       </c>
       <c r="Q26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.7763340025902341E-2</v>
       </c>
       <c r="R26" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25852228066912319</v>
       </c>
       <c r="T26" s="34"/>
@@ -5323,7 +5326,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" ref="A27:A30" si="1">A26+1</f>
+        <f t="shared" ref="A27:A30" si="2">A26+1</f>
         <v>2</v>
       </c>
       <c r="C27" s="15">
@@ -5331,63 +5334,63 @@
         <v>0.19751783979247906</v>
       </c>
       <c r="D27" s="15">
-        <f t="shared" ref="D27:R27" si="2">(D8/D9)-1</f>
+        <f t="shared" ref="D27:R27" si="3">(D8/D9)-1</f>
         <v>-9.276436666696275E-2</v>
       </c>
       <c r="E27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1698938401325076E-2</v>
       </c>
       <c r="F27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5.9032691128102055E-2</v>
       </c>
       <c r="G27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.6753767380775439E-2</v>
       </c>
       <c r="H27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4221794072617753E-2</v>
       </c>
       <c r="I27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-4.3140747587474548E-2</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.10280391950165912</v>
       </c>
       <c r="K27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.6766206269346235E-2</v>
       </c>
       <c r="L27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-9.2545168457396798E-2</v>
       </c>
       <c r="M27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3.9219342480681485E-2</v>
       </c>
       <c r="N27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.18908855007090697</v>
       </c>
       <c r="O27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24984082909823457</v>
       </c>
       <c r="P27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.14188101151990107</v>
       </c>
       <c r="Q27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.10721056495603187</v>
       </c>
       <c r="R27" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.18010938619017747</v>
       </c>
       <c r="T27" s="15"/>
@@ -5401,7 +5404,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C28" s="15">
@@ -5409,63 +5412,63 @@
         <v>0.25646268672830819</v>
       </c>
       <c r="D28" s="15">
-        <f t="shared" ref="D28:R28" si="3">(D11/D12)-1</f>
+        <f t="shared" ref="D28:R28" si="4">(D11/D12)-1</f>
         <v>-8.8491683697801138E-3</v>
       </c>
       <c r="E28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.3840254470228563E-2</v>
       </c>
       <c r="F28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.1317383830811063E-2</v>
       </c>
       <c r="G28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3.1905172992594988E-2</v>
       </c>
       <c r="H28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.2260209641986632E-2</v>
       </c>
       <c r="I28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.913781536360637E-2</v>
       </c>
       <c r="J28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.10205138645053313</v>
       </c>
       <c r="K28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.3710136465821319E-2</v>
       </c>
       <c r="L28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4.7758610082039299E-3</v>
       </c>
       <c r="M28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-6.8334115734363099E-3</v>
       </c>
       <c r="N28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.18277773424703936</v>
       </c>
       <c r="O28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-1.3312773550577583E-2</v>
       </c>
       <c r="P28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-6.2561852170983534E-2</v>
       </c>
       <c r="Q28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-5.8890452041020835E-2</v>
       </c>
       <c r="R28" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.1669857489501978</v>
       </c>
       <c r="T28" s="15"/>
@@ -5479,7 +5482,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C29" s="15">
@@ -5487,63 +5490,63 @@
         <v>2.2617581670861808E-2</v>
       </c>
       <c r="D29" s="15">
-        <f t="shared" ref="D29:R29" si="4">(D14/D15)-1</f>
+        <f t="shared" ref="D29:R29" si="5">(D14/D15)-1</f>
         <v>-1.0808853999729751E-3</v>
       </c>
       <c r="E29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8306416665261578E-2</v>
       </c>
       <c r="F29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.1999354749875355E-3</v>
       </c>
       <c r="G29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.1917326009136531E-2</v>
       </c>
       <c r="H29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0016609646382761E-2</v>
       </c>
       <c r="I29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.5923299143229244E-2</v>
       </c>
       <c r="J29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-3.385898197895254E-2</v>
       </c>
       <c r="K29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.10476866889154923</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.696950280521996E-2</v>
       </c>
       <c r="M29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-8.3030329097429356E-2</v>
       </c>
       <c r="N29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.14078501293855417</v>
       </c>
       <c r="O29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.15861999003068639</v>
       </c>
       <c r="P29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-6.7326038437284574E-2</v>
       </c>
       <c r="Q29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.10523703005015461</v>
       </c>
       <c r="R29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.24930036235826813</v>
       </c>
       <c r="T29" s="15"/>
@@ -5557,7 +5560,7 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C30" s="15">
@@ -5565,63 +5568,63 @@
         <v>7.3143376976864793E-2</v>
       </c>
       <c r="D30" s="15">
-        <f t="shared" ref="D30:R30" si="5">(D17/D18)-1</f>
+        <f t="shared" ref="D30:R30" si="6">(D17/D18)-1</f>
         <v>-8.3641311857414191E-2</v>
       </c>
       <c r="E30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-5.1515123253855766E-3</v>
       </c>
       <c r="F30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.3094188465290033E-2</v>
       </c>
       <c r="G30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.12294637825966181</v>
       </c>
       <c r="H30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.22275591448484011</v>
       </c>
       <c r="I30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.1350861922453204E-2</v>
       </c>
       <c r="J30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.10377296264968261</v>
       </c>
       <c r="K30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.5478618546968193E-2</v>
       </c>
       <c r="L30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.1459923244266941E-2</v>
       </c>
       <c r="M30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.16501618699201137</v>
       </c>
       <c r="N30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.20763657163752081</v>
       </c>
       <c r="O30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.15441602399973542</v>
       </c>
       <c r="P30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-9.2363423757613416E-2</v>
       </c>
       <c r="Q30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.10786277277313128</v>
       </c>
       <c r="R30" s="15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1508407556542597E-2</v>
       </c>
       <c r="T30" s="15"/>
@@ -5655,6 +5658,78 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
+    <cfRule type="colorScale" priority="104">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D3">
+    <cfRule type="colorScale" priority="103">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E3">
+    <cfRule type="colorScale" priority="102">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F3">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G3">
+    <cfRule type="colorScale" priority="100">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule type="colorScale" priority="99">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="colorScale" priority="98">
       <colorScale>
         <cfvo type="min"/>
@@ -5666,7 +5741,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
@@ -5678,7 +5753,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3">
+  <conditionalFormatting sqref="K2:K3">
     <cfRule type="colorScale" priority="96">
       <colorScale>
         <cfvo type="min"/>
@@ -5690,7 +5765,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F3">
+  <conditionalFormatting sqref="L2:L3">
     <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
@@ -5702,7 +5777,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="M2:M3">
     <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min"/>
@@ -5714,7 +5789,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="N2:N3">
     <cfRule type="colorScale" priority="93">
       <colorScale>
         <cfvo type="min"/>
@@ -5726,7 +5801,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="O2:O3">
     <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min"/>
@@ -5738,7 +5813,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="P2:P3">
     <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
@@ -5750,7 +5825,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K3">
+  <conditionalFormatting sqref="Q2:Q3">
     <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>
@@ -5762,7 +5837,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L3">
+  <conditionalFormatting sqref="R2:R3">
     <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
@@ -5774,31 +5849,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M3">
-    <cfRule type="colorScale" priority="88">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N3">
-    <cfRule type="colorScale" priority="87">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O3">
+  <conditionalFormatting sqref="C5:C6">
     <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
@@ -5810,7 +5861,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P3">
+  <conditionalFormatting sqref="D5:D6">
     <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
@@ -5822,7 +5873,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q3">
+  <conditionalFormatting sqref="E5:E6">
     <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
@@ -5834,7 +5885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R3">
+  <conditionalFormatting sqref="F5:F6">
     <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
@@ -5846,7 +5897,31 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C6">
+  <conditionalFormatting sqref="G5:G6">
+    <cfRule type="colorScale" priority="82">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I6">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
@@ -5858,7 +5933,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D6">
+  <conditionalFormatting sqref="J5:J6">
     <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
@@ -5870,7 +5945,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E6">
+  <conditionalFormatting sqref="K5:K6">
     <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
@@ -5882,7 +5957,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:F6">
+  <conditionalFormatting sqref="L5:L6">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
@@ -5894,7 +5969,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G6">
+  <conditionalFormatting sqref="M5:M6">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
@@ -5906,7 +5981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H6">
+  <conditionalFormatting sqref="N5:N6">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -5918,7 +5993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:I6">
+  <conditionalFormatting sqref="O5:O6">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
@@ -5930,7 +6005,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:J6">
+  <conditionalFormatting sqref="P5:P6">
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
@@ -5942,7 +6017,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K6">
+  <conditionalFormatting sqref="Q5:Q6">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
@@ -5954,7 +6029,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:L6">
+  <conditionalFormatting sqref="R5:R6">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
@@ -5966,7 +6041,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M5:M6">
+  <conditionalFormatting sqref="C8:C9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -5978,7 +6053,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5:N6">
+  <conditionalFormatting sqref="D8:D9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -5990,7 +6065,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5:O6">
+  <conditionalFormatting sqref="E8:E9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -6002,7 +6077,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P5:P6">
+  <conditionalFormatting sqref="F8:F9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
         <cfvo type="min"/>
@@ -6014,7 +6089,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5:Q6">
+  <conditionalFormatting sqref="G8:G9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -6026,7 +6101,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R5:R6">
+  <conditionalFormatting sqref="H8:H9">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -6038,7 +6113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C9">
+  <conditionalFormatting sqref="I8:I9">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -6050,7 +6125,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
+  <conditionalFormatting sqref="J8:J9">
     <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
@@ -6062,7 +6137,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E9">
+  <conditionalFormatting sqref="K8:K9">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -6074,7 +6149,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8:F9">
+  <conditionalFormatting sqref="L8:L9">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -6086,7 +6161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G9">
+  <conditionalFormatting sqref="M8:M9">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -6098,7 +6173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8:H9">
+  <conditionalFormatting sqref="N8:N9">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -6110,7 +6185,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I9">
+  <conditionalFormatting sqref="O8:O9">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -6122,7 +6197,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J8:J9">
+  <conditionalFormatting sqref="P8:P9">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -6134,7 +6209,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K9">
+  <conditionalFormatting sqref="Q8:Q9">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -6146,7 +6221,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:L9">
+  <conditionalFormatting sqref="R8:R9">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -6158,7 +6233,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:M9">
+  <conditionalFormatting sqref="C11:C12">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -6170,7 +6245,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N8:N9">
+  <conditionalFormatting sqref="D11:D12">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -6182,7 +6257,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O9">
+  <conditionalFormatting sqref="E11:E12">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -6194,7 +6269,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:P9">
+  <conditionalFormatting sqref="F11:F12">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -6206,7 +6281,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q8:Q9">
+  <conditionalFormatting sqref="G11:G12">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -6218,7 +6293,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R8:R9">
+  <conditionalFormatting sqref="H11:H12">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -6230,7 +6305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
+  <conditionalFormatting sqref="I11:I12">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -6242,7 +6317,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D12">
+  <conditionalFormatting sqref="C14:C15">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -6254,7 +6329,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E12">
+  <conditionalFormatting sqref="D14:D15">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -6266,7 +6341,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11:F12">
+  <conditionalFormatting sqref="E14:E15">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -6278,7 +6353,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11:G12">
+  <conditionalFormatting sqref="F14:F15">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -6290,7 +6365,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H12">
+  <conditionalFormatting sqref="G14:G15">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -6302,7 +6377,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I11:I12">
+  <conditionalFormatting sqref="J11:J12">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -6314,7 +6389,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C15">
+  <conditionalFormatting sqref="K11:K12">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -6326,7 +6401,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D15">
+  <conditionalFormatting sqref="L11:L12">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -6338,7 +6413,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E15">
+  <conditionalFormatting sqref="M11:M12">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -6350,7 +6425,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F15">
+  <conditionalFormatting sqref="N11:N12">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -6362,7 +6437,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:G15">
+  <conditionalFormatting sqref="O11:O12">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -6374,7 +6449,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J12">
+  <conditionalFormatting sqref="P11:P12">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -6386,7 +6461,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K12">
+  <conditionalFormatting sqref="Q11:Q12">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -6398,7 +6473,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L11:L12">
+  <conditionalFormatting sqref="R11:R12">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -6410,7 +6485,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M11:M12">
+  <conditionalFormatting sqref="H14:H15">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -6422,7 +6497,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N11:N12">
+  <conditionalFormatting sqref="I14:I15">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -6434,7 +6509,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O11:O12">
+  <conditionalFormatting sqref="J14:J15">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -6446,7 +6521,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11:P12">
+  <conditionalFormatting sqref="K14:K15">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -6458,7 +6533,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q11:Q12">
+  <conditionalFormatting sqref="L14:L15">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -6470,7 +6545,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R11:R12">
+  <conditionalFormatting sqref="M14:M15">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -6482,7 +6557,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H15">
+  <conditionalFormatting sqref="N14:N15">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -6494,7 +6569,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I15">
+  <conditionalFormatting sqref="O14:O15">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -6506,7 +6581,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J15">
+  <conditionalFormatting sqref="P14:P15">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -6518,7 +6593,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K14:K15">
+  <conditionalFormatting sqref="Q14:Q15">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -6530,7 +6605,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14:L15">
+  <conditionalFormatting sqref="R14:R15">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -6542,7 +6617,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M15">
+  <conditionalFormatting sqref="R17:R18">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -6554,7 +6629,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14:N15">
+  <conditionalFormatting sqref="C17:C18">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -6566,7 +6641,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O14:O15">
+  <conditionalFormatting sqref="D17:D18">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -6578,7 +6653,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P14:P15">
+  <conditionalFormatting sqref="E17:E18">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -6590,7 +6665,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q14:Q15">
+  <conditionalFormatting sqref="F17:F18">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -6602,7 +6677,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R14:R15">
+  <conditionalFormatting sqref="G17:G18">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -6614,7 +6689,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R17:R18">
+  <conditionalFormatting sqref="H17:H18">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -6626,7 +6701,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C18">
+  <conditionalFormatting sqref="I17:I18">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -6638,7 +6713,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D18">
+  <conditionalFormatting sqref="J17:J18">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -6650,7 +6725,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17:E18">
+  <conditionalFormatting sqref="K17:K18">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -6662,7 +6737,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F18">
+  <conditionalFormatting sqref="L17:L18">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -6674,7 +6749,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G17:G18">
+  <conditionalFormatting sqref="M17:M18">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -6686,7 +6761,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H18">
+  <conditionalFormatting sqref="N17:N18">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -6698,7 +6773,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17:I18">
+  <conditionalFormatting sqref="O17:O18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -6710,7 +6785,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17:J18">
+  <conditionalFormatting sqref="P17:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -6722,7 +6797,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17:K18">
+  <conditionalFormatting sqref="Q17:Q18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -6734,7 +6809,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17:L18">
+  <conditionalFormatting sqref="C25:R25">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -6746,7 +6821,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:M18">
+  <conditionalFormatting sqref="C26:R26">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -6758,7 +6833,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17:N18">
+  <conditionalFormatting sqref="C27:R27">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6770,7 +6845,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O18">
+  <conditionalFormatting sqref="C28:R28">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -6782,7 +6857,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P17:P18">
+  <conditionalFormatting sqref="C29:R29">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -6794,7 +6869,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17:Q18">
+  <conditionalFormatting sqref="C30:R30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>